<commit_message>
updating stressor trait sensitivities/ad caps, adding larger species list
</commit_message>
<xml_diff>
--- a/trait_stressor_rankings/trait_stressor_adcap_general.xlsx
+++ b/trait_stressor_rankings/trait_stressor_adcap_general.xlsx
@@ -10,7 +10,7 @@
     <sheet name="stressor1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="adcap_traits_1" localSheetId="0">stressor1!$D$2:$E$76</definedName>
+    <definedName name="adcap_traits_1" localSheetId="0">stressor1!$D$2:$E$77</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="86">
   <si>
     <t>no</t>
   </si>
@@ -284,13 +284,16 @@
     <t>why is "does not aggregate" here in foraging range?</t>
   </si>
   <si>
-    <t>is this redundant with lifetime # of reproductive opportunities X age to first reproduction?</t>
-  </si>
-  <si>
     <t>these general adaptive capacity things seem to be more about the population's adaptive capacity rather than individual…</t>
   </si>
   <si>
     <t>based on notes from other spreadsheet; but are these always valid? Sexual dioecious is probably better for genetic diversity</t>
+  </si>
+  <si>
+    <t>&lt;1</t>
+  </si>
+  <si>
+    <t>This relates to exposure over a lifetime.  A species with long life and few opportunities is more vulnerable than one with a short life and few opportunities</t>
   </si>
 </sst>
 </file>
@@ -390,7 +393,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -400,8 +403,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -426,17 +433,20 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -770,10 +780,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E75"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -815,7 +825,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -877,7 +887,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -933,7 +943,7 @@
         <v>53</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="D10" s="18">
         <v>0</v>
@@ -948,10 +958,10 @@
         <v>53</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D11" s="18">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E11" s="5"/>
     </row>
@@ -963,10 +973,10 @@
         <v>53</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D12" s="18">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E12" s="5"/>
     </row>
@@ -978,10 +988,10 @@
         <v>53</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D13" s="18">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E13" s="5"/>
     </row>
@@ -993,10 +1003,10 @@
         <v>53</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D14" s="18">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="E14" s="5"/>
     </row>
@@ -1008,10 +1018,10 @@
         <v>53</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D15" s="18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E15" s="5"/>
     </row>
@@ -1023,10 +1033,10 @@
         <v>53</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D16" s="18">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="E16" s="5"/>
     </row>
@@ -1038,10 +1048,10 @@
         <v>53</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D17" s="18">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="E17" s="5"/>
     </row>
@@ -1053,10 +1063,10 @@
         <v>53</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D18" s="18">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="E18" s="5"/>
     </row>
@@ -1064,16 +1074,16 @@
       <c r="A19" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D19" s="17">
-        <v>0</v>
-      </c>
-      <c r="E19" s="8"/>
+      <c r="B19" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="18">
+        <v>1</v>
+      </c>
+      <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="7" t="s">
@@ -1083,10 +1093,10 @@
         <v>46</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D20" s="17">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="E20" s="8"/>
     </row>
@@ -1098,10 +1108,10 @@
         <v>46</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D21" s="17">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="E21" s="8"/>
     </row>
@@ -1113,10 +1123,10 @@
         <v>46</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D22" s="17">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="E22" s="8"/>
     </row>
@@ -1128,10 +1138,10 @@
         <v>46</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D23" s="17">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="E23" s="8"/>
     </row>
@@ -1143,10 +1153,10 @@
         <v>46</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D24" s="17">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="E24" s="8"/>
     </row>
@@ -1154,16 +1164,16 @@
       <c r="A25" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D25" s="18">
-        <v>0</v>
-      </c>
-      <c r="E25" s="5"/>
+      <c r="B25" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" s="17">
+        <v>1</v>
+      </c>
+      <c r="E25" s="8"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="7" t="s">
@@ -1173,10 +1183,10 @@
         <v>43</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D26" s="18">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="E26" s="5"/>
     </row>
@@ -1188,10 +1198,10 @@
         <v>43</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D27" s="18">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="E27" s="5"/>
     </row>
@@ -1203,10 +1213,10 @@
         <v>43</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D28" s="18">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="E28" s="5"/>
     </row>
@@ -1218,114 +1228,134 @@
         <v>43</v>
       </c>
       <c r="C29" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" s="18">
+        <v>0.75</v>
+      </c>
+      <c r="E29" s="5"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D29" s="18">
-        <v>1</v>
-      </c>
-      <c r="E29" s="5"/>
-    </row>
-    <row r="30" spans="1:5" s="14" customFormat="1">
-      <c r="A30" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B30" s="13" t="s">
+      <c r="D30" s="18">
+        <v>1</v>
+      </c>
+      <c r="E30" s="5"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C31" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D30" s="20"/>
-      <c r="E30" s="24" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" s="14" customFormat="1">
-      <c r="A31" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B31" s="13" t="s">
+      <c r="D31" s="17">
+        <v>0</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C32" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D31" s="20"/>
-    </row>
-    <row r="32" spans="1:5" s="14" customFormat="1">
-      <c r="A32" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B32" s="13" t="s">
+      <c r="D32" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="E32" s="8"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C33" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D32" s="20"/>
-    </row>
-    <row r="33" spans="1:5" s="14" customFormat="1">
-      <c r="A33" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B33" s="13" t="s">
+      <c r="D33" s="17">
+        <v>0.3</v>
+      </c>
+      <c r="E33" s="8"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C34" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D33" s="20"/>
-    </row>
-    <row r="34" spans="1:5" s="14" customFormat="1">
-      <c r="A34" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B34" s="13" t="s">
+      <c r="D34" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="E34" s="8"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C35" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D34" s="20"/>
-    </row>
-    <row r="35" spans="1:5" s="14" customFormat="1">
-      <c r="A35" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B35" s="13" t="s">
+      <c r="D35" s="17">
+        <v>0.7</v>
+      </c>
+      <c r="E35" s="8"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B36" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C36" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D35" s="20"/>
-    </row>
-    <row r="36" spans="1:5" s="14" customFormat="1">
-      <c r="A36" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B36" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="D36" s="20"/>
+      <c r="D36" s="17">
+        <v>0.9</v>
+      </c>
+      <c r="E36" s="8"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B37" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D37" s="18">
-        <v>0</v>
-      </c>
-      <c r="E37" s="5"/>
+      <c r="B37" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D37" s="17">
+        <v>1</v>
+      </c>
+      <c r="E37" s="8"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="7" t="s">
@@ -1335,10 +1365,10 @@
         <v>31</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D38" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E38" s="5"/>
     </row>
@@ -1350,10 +1380,10 @@
         <v>31</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D39" s="18">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E39" s="5"/>
     </row>
@@ -1361,16 +1391,16 @@
       <c r="A40" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B40" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D40" s="17">
-        <v>0</v>
-      </c>
-      <c r="E40" s="8"/>
+      <c r="B40" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D40" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="E40" s="5"/>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="7" t="s">
@@ -1380,10 +1410,10 @@
         <v>25</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D41" s="17">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="E41" s="8"/>
     </row>
@@ -1395,10 +1425,10 @@
         <v>25</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D42" s="17">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="E42" s="8"/>
     </row>
@@ -1410,10 +1440,10 @@
         <v>25</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D43" s="17">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="E43" s="8"/>
     </row>
@@ -1425,29 +1455,29 @@
         <v>25</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="D44" s="17">
-        <v>1</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>79</v>
-      </c>
+        <v>0.75</v>
+      </c>
+      <c r="E44" s="8"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B45" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D45" s="18">
-        <v>0</v>
-      </c>
-      <c r="E45" s="5"/>
+      <c r="B45" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45" s="17">
+        <v>1</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="7" t="s">
@@ -1457,10 +1487,10 @@
         <v>20</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D46" s="18">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="E46" s="5"/>
     </row>
@@ -1472,10 +1502,10 @@
         <v>20</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D47" s="18">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="E47" s="5"/>
     </row>
@@ -1487,10 +1517,10 @@
         <v>20</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D48" s="18">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="E48" s="5"/>
     </row>
@@ -1502,10 +1532,10 @@
         <v>20</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D49" s="18">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="E49" s="5"/>
     </row>
@@ -1513,16 +1543,16 @@
       <c r="A50" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B50" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D50" s="17">
-        <v>1</v>
-      </c>
-      <c r="E50" s="8"/>
+      <c r="B50" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D50" s="18">
+        <v>1</v>
+      </c>
+      <c r="E50" s="5"/>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="7" t="s">
@@ -1532,27 +1562,27 @@
         <v>18</v>
       </c>
       <c r="C51" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D51" s="17">
+        <v>1</v>
+      </c>
+      <c r="E51" s="8"/>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C52" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D51" s="17">
+      <c r="D52" s="17">
         <v>0</v>
       </c>
-      <c r="E51" s="8"/>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D52" s="19">
-        <v>0</v>
-      </c>
-      <c r="E52" s="3"/>
+      <c r="E52" s="8"/>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="4" t="s">
@@ -1562,10 +1592,10 @@
         <v>16</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D53" s="19">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E53" s="3"/>
     </row>
@@ -1577,10 +1607,10 @@
         <v>16</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D54" s="19">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E54" s="3"/>
     </row>
@@ -1592,7 +1622,7 @@
         <v>16</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D55" s="19">
         <v>1</v>
@@ -1607,28 +1637,28 @@
         <v>16</v>
       </c>
       <c r="C56" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D56" s="19">
+        <v>1</v>
+      </c>
+      <c r="E56" s="3"/>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C57" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D56" s="19" t="s">
+      <c r="D57" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E56" s="3" t="s">
+      <c r="E57" s="3" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" s="14" customFormat="1">
-      <c r="A57" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B57" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C57" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D57" s="20"/>
-      <c r="E57" s="14" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="58" spans="1:5" s="14" customFormat="1">
@@ -1639,9 +1669,12 @@
         <v>5</v>
       </c>
       <c r="C58" s="13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D58" s="20"/>
+      <c r="E58" s="14" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="59" spans="1:5" s="14" customFormat="1">
       <c r="A59" s="13" t="s">
@@ -1651,7 +1684,7 @@
         <v>5</v>
       </c>
       <c r="C59" s="13" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D59" s="20"/>
     </row>
@@ -1663,7 +1696,7 @@
         <v>5</v>
       </c>
       <c r="C60" s="13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D60" s="20"/>
     </row>
@@ -1675,26 +1708,23 @@
         <v>5</v>
       </c>
       <c r="C61" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D61" s="20"/>
+    </row>
+    <row r="62" spans="1:5" s="14" customFormat="1">
+      <c r="A62" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B62" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D61" s="20" t="s">
+      <c r="D62" s="20" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="62" spans="1:5">
-      <c r="A62" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D62" s="19">
-        <v>0</v>
-      </c>
-      <c r="E62" s="3"/>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="4" t="s">
@@ -1704,27 +1734,27 @@
         <v>1</v>
       </c>
       <c r="C63" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D63" s="19">
         <v>0</v>
       </c>
-      <c r="D63" s="19">
-        <v>1</v>
-      </c>
       <c r="E63" s="3"/>
     </row>
     <row r="64" spans="1:5">
-      <c r="A64" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D64" s="21">
+      <c r="A64" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C64" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E64" s="1"/>
+      <c r="D64" s="19">
+        <v>1</v>
+      </c>
+      <c r="E64" s="3"/>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="2" t="s">
@@ -1734,10 +1764,10 @@
         <v>10</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D65" s="21">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E65" s="1"/>
     </row>
@@ -1749,60 +1779,60 @@
         <v>10</v>
       </c>
       <c r="C66" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D66" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="E66" s="1"/>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C67" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D66" s="21">
-        <v>1</v>
-      </c>
-      <c r="E66" s="1"/>
-    </row>
-    <row r="67" spans="1:5" s="14" customFormat="1">
-      <c r="A67" s="13" t="s">
+      <c r="D67" s="21">
+        <v>1</v>
+      </c>
+      <c r="E67" s="1"/>
+    </row>
+    <row r="68" spans="1:5" s="14" customFormat="1">
+      <c r="A68" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B67" s="13" t="s">
+      <c r="B68" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C67" s="13" t="s">
+      <c r="C68" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D67" s="20">
-        <v>1</v>
-      </c>
-      <c r="E67" s="14" t="s">
+      <c r="D68" s="20">
+        <v>1</v>
+      </c>
+      <c r="E68" s="14" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
-      <c r="A68" s="2" t="s">
+    <row r="69" spans="1:5">
+      <c r="A69" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B69" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="C69" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D68" s="21" t="s">
+      <c r="D69" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E68" s="1" t="s">
+      <c r="E69" s="1" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" s="14" customFormat="1">
-      <c r="A69" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B69" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C69" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D69" s="20"/>
-      <c r="E69" s="14" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="70" spans="1:5" s="14" customFormat="1">
@@ -1813,9 +1843,12 @@
         <v>5</v>
       </c>
       <c r="C70" s="13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D70" s="20"/>
+      <c r="E70" s="14" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="71" spans="1:5" s="14" customFormat="1">
       <c r="A71" s="13" t="s">
@@ -1825,7 +1858,7 @@
         <v>5</v>
       </c>
       <c r="C71" s="13" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D71" s="20"/>
     </row>
@@ -1837,7 +1870,7 @@
         <v>5</v>
       </c>
       <c r="C72" s="13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D72" s="20"/>
     </row>
@@ -1849,26 +1882,23 @@
         <v>5</v>
       </c>
       <c r="C73" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D73" s="20"/>
+    </row>
+    <row r="74" spans="1:5" s="14" customFormat="1">
+      <c r="A74" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B74" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C74" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D73" s="20" t="s">
+      <c r="D74" s="20" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="74" spans="1:5">
-      <c r="A74" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D74" s="21">
-        <v>0</v>
-      </c>
-      <c r="E74" s="1"/>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="2" t="s">
@@ -1878,12 +1908,27 @@
         <v>1</v>
       </c>
       <c r="C75" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D75" s="21">
         <v>0</v>
       </c>
-      <c r="D75" s="21">
-        <v>1</v>
-      </c>
       <c r="E75" s="1"/>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D76" s="21">
+        <v>1</v>
+      </c>
+      <c r="E76" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
breaking out expert sheets into csvs for github version control and editing
</commit_message>
<xml_diff>
--- a/trait_stressor_rankings/trait_stressor_adcap_general.xlsx
+++ b/trait_stressor_rankings/trait_stressor_adcap_general.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4120" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="2120" yWindow="120" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="stressor1" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="90">
   <si>
     <t>no</t>
   </si>
@@ -294,6 +294,18 @@
   </si>
   <si>
     <t>This relates to exposure over a lifetime.  A species with long life and few opportunities is more vulnerable than one with a short life and few opportunities</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>lit review</t>
   </si>
 </sst>
 </file>
@@ -782,8 +794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -821,8 +833,8 @@
       <c r="C2" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="16">
-        <v>0</v>
+      <c r="D2" s="16" t="s">
+        <v>86</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>82</v>
@@ -838,8 +850,8 @@
       <c r="C3" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="D3" s="16">
-        <v>0.25</v>
+      <c r="D3" s="16" t="s">
+        <v>87</v>
       </c>
       <c r="E3" s="9"/>
     </row>
@@ -853,8 +865,8 @@
       <c r="C4" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D4" s="16">
-        <v>0.5</v>
+      <c r="D4" s="16" t="s">
+        <v>7</v>
       </c>
       <c r="E4" s="9"/>
     </row>
@@ -868,8 +880,8 @@
       <c r="C5" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="D5" s="16">
-        <v>1</v>
+      <c r="D5" s="16" t="s">
+        <v>88</v>
       </c>
       <c r="E5" s="9"/>
     </row>
@@ -883,8 +895,8 @@
       <c r="C6" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D6" s="17">
-        <v>0</v>
+      <c r="D6" s="17" t="s">
+        <v>87</v>
       </c>
       <c r="E6" s="23" t="s">
         <v>83</v>
@@ -900,10 +912,12 @@
       <c r="C7" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="17">
-        <v>0.5</v>
-      </c>
-      <c r="E7" s="8"/>
+      <c r="D7" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="7" t="s">
@@ -915,8 +929,8 @@
       <c r="C8" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D8" s="17">
-        <v>1</v>
+      <c r="D8" s="17" t="s">
+        <v>88</v>
       </c>
       <c r="E8" s="8"/>
     </row>
@@ -930,8 +944,8 @@
       <c r="C9" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="17">
-        <v>1</v>
+      <c r="D9" s="17" t="s">
+        <v>88</v>
       </c>
       <c r="E9" s="8"/>
     </row>
@@ -945,8 +959,8 @@
       <c r="C10" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="D10" s="18">
-        <v>0</v>
+      <c r="D10" s="18" t="s">
+        <v>86</v>
       </c>
       <c r="E10" s="5"/>
     </row>
@@ -960,8 +974,8 @@
       <c r="C11" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="18">
-        <v>0</v>
+      <c r="D11" s="18" t="s">
+        <v>86</v>
       </c>
       <c r="E11" s="5"/>
     </row>
@@ -975,8 +989,8 @@
       <c r="C12" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="18">
-        <v>0.1</v>
+      <c r="D12" s="18" t="s">
+        <v>87</v>
       </c>
       <c r="E12" s="5"/>
     </row>
@@ -990,8 +1004,8 @@
       <c r="C13" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="18">
-        <v>0.2</v>
+      <c r="D13" s="18" t="s">
+        <v>87</v>
       </c>
       <c r="E13" s="5"/>
     </row>
@@ -1005,8 +1019,8 @@
       <c r="C14" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D14" s="18">
-        <v>0.3</v>
+      <c r="D14" s="18" t="s">
+        <v>87</v>
       </c>
       <c r="E14" s="5"/>
     </row>
@@ -1020,8 +1034,8 @@
       <c r="C15" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="18">
-        <v>0.4</v>
+      <c r="D15" s="18" t="s">
+        <v>7</v>
       </c>
       <c r="E15" s="5"/>
     </row>
@@ -1035,8 +1049,8 @@
       <c r="C16" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="18">
-        <v>0.5</v>
+      <c r="D16" s="18" t="s">
+        <v>7</v>
       </c>
       <c r="E16" s="5"/>
     </row>
@@ -1050,8 +1064,8 @@
       <c r="C17" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D17" s="18">
-        <v>0.6</v>
+      <c r="D17" s="18" t="s">
+        <v>7</v>
       </c>
       <c r="E17" s="5"/>
     </row>
@@ -1065,8 +1079,8 @@
       <c r="C18" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="18">
-        <v>0.8</v>
+      <c r="D18" s="18" t="s">
+        <v>88</v>
       </c>
       <c r="E18" s="5"/>
     </row>
@@ -1080,8 +1094,8 @@
       <c r="C19" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D19" s="18">
-        <v>1</v>
+      <c r="D19" s="18" t="s">
+        <v>88</v>
       </c>
       <c r="E19" s="5"/>
     </row>
@@ -1095,8 +1109,8 @@
       <c r="C20" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="17">
-        <v>0</v>
+      <c r="D20" s="17" t="s">
+        <v>86</v>
       </c>
       <c r="E20" s="8"/>
     </row>
@@ -1110,8 +1124,8 @@
       <c r="C21" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="17">
-        <v>0.2</v>
+      <c r="D21" s="17" t="s">
+        <v>87</v>
       </c>
       <c r="E21" s="8"/>
     </row>
@@ -1125,8 +1139,8 @@
       <c r="C22" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="17">
-        <v>0.4</v>
+      <c r="D22" s="17" t="s">
+        <v>87</v>
       </c>
       <c r="E22" s="8"/>
     </row>
@@ -1140,8 +1154,8 @@
       <c r="C23" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="17">
-        <v>0.6</v>
+      <c r="D23" s="17" t="s">
+        <v>7</v>
       </c>
       <c r="E23" s="8"/>
     </row>
@@ -1155,8 +1169,8 @@
       <c r="C24" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="17">
-        <v>0.8</v>
+      <c r="D24" s="17" t="s">
+        <v>7</v>
       </c>
       <c r="E24" s="8"/>
     </row>
@@ -1170,8 +1184,8 @@
       <c r="C25" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D25" s="17">
-        <v>1</v>
+      <c r="D25" s="17" t="s">
+        <v>88</v>
       </c>
       <c r="E25" s="8"/>
     </row>
@@ -1185,8 +1199,8 @@
       <c r="C26" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D26" s="18">
-        <v>0</v>
+      <c r="D26" s="18" t="s">
+        <v>86</v>
       </c>
       <c r="E26" s="5"/>
     </row>
@@ -1200,8 +1214,8 @@
       <c r="C27" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="18">
-        <v>0.25</v>
+      <c r="D27" s="18" t="s">
+        <v>87</v>
       </c>
       <c r="E27" s="5"/>
     </row>
@@ -1215,8 +1229,8 @@
       <c r="C28" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D28" s="18">
-        <v>0.5</v>
+      <c r="D28" s="18" t="s">
+        <v>87</v>
       </c>
       <c r="E28" s="5"/>
     </row>
@@ -1230,8 +1244,8 @@
       <c r="C29" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D29" s="18">
-        <v>0.75</v>
+      <c r="D29" s="18" t="s">
+        <v>7</v>
       </c>
       <c r="E29" s="5"/>
     </row>
@@ -1245,8 +1259,8 @@
       <c r="C30" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D30" s="18">
-        <v>1</v>
+      <c r="D30" s="18" t="s">
+        <v>88</v>
       </c>
       <c r="E30" s="5"/>
     </row>
@@ -1260,8 +1274,8 @@
       <c r="C31" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="17">
-        <v>0</v>
+      <c r="D31" s="17" t="s">
+        <v>86</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>85</v>
@@ -1277,8 +1291,8 @@
       <c r="C32" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D32" s="17">
-        <v>0.1</v>
+      <c r="D32" s="17" t="s">
+        <v>87</v>
       </c>
       <c r="E32" s="8"/>
     </row>
@@ -1292,8 +1306,8 @@
       <c r="C33" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D33" s="17">
-        <v>0.3</v>
+      <c r="D33" s="17" t="s">
+        <v>87</v>
       </c>
       <c r="E33" s="8"/>
     </row>
@@ -1307,8 +1321,8 @@
       <c r="C34" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D34" s="17">
-        <v>0.5</v>
+      <c r="D34" s="17" t="s">
+        <v>7</v>
       </c>
       <c r="E34" s="8"/>
     </row>
@@ -1322,8 +1336,8 @@
       <c r="C35" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D35" s="17">
-        <v>0.7</v>
+      <c r="D35" s="17" t="s">
+        <v>7</v>
       </c>
       <c r="E35" s="8"/>
     </row>
@@ -1337,8 +1351,8 @@
       <c r="C36" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D36" s="17">
-        <v>0.9</v>
+      <c r="D36" s="17" t="s">
+        <v>88</v>
       </c>
       <c r="E36" s="8"/>
     </row>
@@ -1352,8 +1366,8 @@
       <c r="C37" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D37" s="17">
-        <v>1</v>
+      <c r="D37" s="17" t="s">
+        <v>88</v>
       </c>
       <c r="E37" s="8"/>
     </row>
@@ -1367,8 +1381,8 @@
       <c r="C38" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D38" s="18">
-        <v>0</v>
+      <c r="D38" s="18" t="s">
+        <v>86</v>
       </c>
       <c r="E38" s="5"/>
     </row>
@@ -1382,8 +1396,8 @@
       <c r="C39" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D39" s="18">
-        <v>1</v>
+      <c r="D39" s="18" t="s">
+        <v>88</v>
       </c>
       <c r="E39" s="5"/>
     </row>
@@ -1397,8 +1411,8 @@
       <c r="C40" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D40" s="18">
-        <v>0.5</v>
+      <c r="D40" s="18" t="s">
+        <v>87</v>
       </c>
       <c r="E40" s="5"/>
     </row>
@@ -1412,8 +1426,8 @@
       <c r="C41" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D41" s="17">
-        <v>0</v>
+      <c r="D41" s="17" t="s">
+        <v>86</v>
       </c>
       <c r="E41" s="8"/>
     </row>
@@ -1427,8 +1441,8 @@
       <c r="C42" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D42" s="17">
-        <v>0.25</v>
+      <c r="D42" s="17" t="s">
+        <v>87</v>
       </c>
       <c r="E42" s="8"/>
     </row>
@@ -1442,8 +1456,8 @@
       <c r="C43" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D43" s="17">
-        <v>0.5</v>
+      <c r="D43" s="17" t="s">
+        <v>7</v>
       </c>
       <c r="E43" s="8"/>
     </row>
@@ -1457,8 +1471,8 @@
       <c r="C44" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D44" s="17">
-        <v>0.75</v>
+      <c r="D44" s="17" t="s">
+        <v>7</v>
       </c>
       <c r="E44" s="8"/>
     </row>
@@ -1472,8 +1486,8 @@
       <c r="C45" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D45" s="17">
-        <v>1</v>
+      <c r="D45" s="17" t="s">
+        <v>88</v>
       </c>
       <c r="E45" s="8" t="s">
         <v>79</v>
@@ -1489,8 +1503,8 @@
       <c r="C46" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D46" s="18">
-        <v>0</v>
+      <c r="D46" s="18" t="s">
+        <v>86</v>
       </c>
       <c r="E46" s="5"/>
     </row>
@@ -1504,8 +1518,8 @@
       <c r="C47" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D47" s="18">
-        <v>0.25</v>
+      <c r="D47" s="18" t="s">
+        <v>87</v>
       </c>
       <c r="E47" s="5"/>
     </row>
@@ -1519,8 +1533,8 @@
       <c r="C48" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D48" s="18">
-        <v>0.5</v>
+      <c r="D48" s="18" t="s">
+        <v>7</v>
       </c>
       <c r="E48" s="5"/>
     </row>
@@ -1534,8 +1548,8 @@
       <c r="C49" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D49" s="18">
-        <v>0.75</v>
+      <c r="D49" s="18" t="s">
+        <v>88</v>
       </c>
       <c r="E49" s="5"/>
     </row>
@@ -1549,8 +1563,8 @@
       <c r="C50" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D50" s="18">
-        <v>1</v>
+      <c r="D50" s="18" t="s">
+        <v>88</v>
       </c>
       <c r="E50" s="5"/>
     </row>
@@ -1564,8 +1578,8 @@
       <c r="C51" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D51" s="17">
-        <v>1</v>
+      <c r="D51" s="17" t="s">
+        <v>88</v>
       </c>
       <c r="E51" s="8"/>
     </row>
@@ -1579,8 +1593,8 @@
       <c r="C52" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D52" s="17">
-        <v>0</v>
+      <c r="D52" s="17" t="s">
+        <v>86</v>
       </c>
       <c r="E52" s="8"/>
     </row>
@@ -1594,8 +1608,8 @@
       <c r="C53" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D53" s="19">
-        <v>0</v>
+      <c r="D53" s="19" t="s">
+        <v>86</v>
       </c>
       <c r="E53" s="3"/>
     </row>
@@ -1609,8 +1623,8 @@
       <c r="C54" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D54" s="19">
-        <v>0.5</v>
+      <c r="D54" s="19" t="s">
+        <v>87</v>
       </c>
       <c r="E54" s="3"/>
     </row>
@@ -1624,8 +1638,8 @@
       <c r="C55" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D55" s="19">
-        <v>1</v>
+      <c r="D55" s="19" t="s">
+        <v>88</v>
       </c>
       <c r="E55" s="3"/>
     </row>
@@ -1639,8 +1653,8 @@
       <c r="C56" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D56" s="19">
-        <v>1</v>
+      <c r="D56" s="19" t="s">
+        <v>88</v>
       </c>
       <c r="E56" s="3"/>
     </row>
@@ -1736,8 +1750,8 @@
       <c r="C63" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D63" s="19">
-        <v>0</v>
+      <c r="D63" s="19" t="s">
+        <v>86</v>
       </c>
       <c r="E63" s="3"/>
     </row>
@@ -1751,8 +1765,8 @@
       <c r="C64" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D64" s="19">
-        <v>1</v>
+      <c r="D64" s="19" t="s">
+        <v>88</v>
       </c>
       <c r="E64" s="3"/>
     </row>
@@ -1766,8 +1780,8 @@
       <c r="C65" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D65" s="21">
-        <v>0</v>
+      <c r="D65" s="21" t="s">
+        <v>86</v>
       </c>
       <c r="E65" s="1"/>
     </row>
@@ -1781,8 +1795,8 @@
       <c r="C66" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D66" s="21">
-        <v>0.5</v>
+      <c r="D66" s="21" t="s">
+        <v>87</v>
       </c>
       <c r="E66" s="1"/>
     </row>
@@ -1796,8 +1810,8 @@
       <c r="C67" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D67" s="21">
-        <v>1</v>
+      <c r="D67" s="21" t="s">
+        <v>88</v>
       </c>
       <c r="E67" s="1"/>
     </row>
@@ -1811,8 +1825,8 @@
       <c r="C68" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D68" s="20">
-        <v>1</v>
+      <c r="D68" s="20" t="s">
+        <v>4</v>
       </c>
       <c r="E68" s="14" t="s">
         <v>81</v>
@@ -1910,8 +1924,8 @@
       <c r="C75" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D75" s="21">
-        <v>0</v>
+      <c r="D75" s="21" t="s">
+        <v>86</v>
       </c>
       <c r="E75" s="1"/>
     </row>
@@ -1925,8 +1939,8 @@
       <c r="C76" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D76" s="21">
-        <v>1</v>
+      <c r="D76" s="21" t="s">
+        <v>88</v>
       </c>
       <c r="E76" s="1"/>
     </row>

</xml_diff>

<commit_message>
identifying weak spots and improving matches
Former-commit-id: b2e14c4666aa59df10b89117a06f9c77a8cfa3c5
</commit_message>
<xml_diff>
--- a/trait_stressor_rankings/trait_stressor_adcap_general.xlsx
+++ b/trait_stressor_rankings/trait_stressor_adcap_general.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2120" yWindow="120" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="4220" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="stressor1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="adcap_traits_1" localSheetId="0">stressor1!$D$2:$E$77</definedName>
+    <definedName name="adcap_traits_1" localSheetId="0">stressor1!$D$2:$E$66</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="84">
   <si>
     <t>no</t>
   </si>
@@ -53,21 +53,9 @@
     <t>NA</t>
   </si>
   <si>
-    <t>if one/few, size</t>
-  </si>
-  <si>
-    <t>large</t>
-  </si>
-  <si>
     <t>medium</t>
   </si>
   <si>
-    <t>small</t>
-  </si>
-  <si>
-    <t>very small</t>
-  </si>
-  <si>
     <t>number of sites, incl. terrestrial wetlands</t>
   </si>
   <si>
@@ -272,16 +260,10 @@
     <t>category</t>
   </si>
   <si>
-    <t>conditional - argh! Can we just drop these? If only one site, doesn't necessarily matter how large</t>
-  </si>
-  <si>
     <t>NA = no dependence</t>
   </si>
   <si>
     <t>is this different from "does not aggregate"?</t>
-  </si>
-  <si>
-    <t>why is "does not aggregate" here in foraging range?</t>
   </si>
   <si>
     <t>these general adaptive capacity things seem to be more about the population's adaptive capacity rather than individual…</t>
@@ -352,7 +334,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -389,12 +371,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -420,7 +396,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -434,14 +410,11 @@
     <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -792,10 +765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E76"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D77" sqref="D77"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -803,1146 +776,999 @@
     <col min="1" max="1" width="53.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="22"/>
+    <col min="4" max="4" width="10.83203125" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="11" customFormat="1">
       <c r="A1" s="12" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>74</v>
+        <v>71</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>70</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="10" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>86</v>
+        <v>68</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>80</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>87</v>
+      <c r="D3" s="14" t="s">
+        <v>81</v>
       </c>
       <c r="E3" s="9"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="10" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>7</v>
+        <v>66</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>5</v>
       </c>
       <c r="E4" s="9"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="10" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>88</v>
+        <v>64</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>82</v>
       </c>
       <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>83</v>
+        <v>62</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>7</v>
+        <v>61</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>5</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>88</v>
+        <v>60</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>82</v>
       </c>
       <c r="E8" s="8"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>88</v>
+        <v>58</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>82</v>
       </c>
       <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>86</v>
+        <v>78</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>80</v>
       </c>
       <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>86</v>
+        <v>57</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>80</v>
       </c>
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>87</v>
+        <v>56</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>81</v>
       </c>
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>87</v>
+        <v>55</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>81</v>
       </c>
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>87</v>
+        <v>54</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>81</v>
       </c>
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B15" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>7</v>
+      <c r="D15" s="16" t="s">
+        <v>5</v>
       </c>
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>7</v>
+        <v>52</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>5</v>
       </c>
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>7</v>
+        <v>51</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>5</v>
       </c>
       <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>88</v>
+        <v>50</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>82</v>
       </c>
       <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>88</v>
+        <v>48</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>82</v>
       </c>
       <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>86</v>
+        <v>47</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>80</v>
       </c>
       <c r="E20" s="8"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B21" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>87</v>
+      <c r="D21" s="15" t="s">
+        <v>81</v>
       </c>
       <c r="E21" s="8"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>87</v>
+        <v>45</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>81</v>
       </c>
       <c r="E22" s="8"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>7</v>
+        <v>44</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>5</v>
       </c>
       <c r="E23" s="8"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>7</v>
+        <v>43</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>5</v>
       </c>
       <c r="E24" s="8"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>88</v>
+        <v>41</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>82</v>
       </c>
       <c r="E25" s="8"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D26" s="18" t="s">
-        <v>86</v>
+        <v>40</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>80</v>
       </c>
       <c r="E26" s="5"/>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D27" s="18" t="s">
-        <v>87</v>
+        <v>35</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>81</v>
       </c>
       <c r="E27" s="5"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D28" s="18" t="s">
-        <v>87</v>
+        <v>34</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>81</v>
       </c>
       <c r="E28" s="5"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D29" s="18" t="s">
-        <v>7</v>
+        <v>33</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>5</v>
       </c>
       <c r="E29" s="5"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D30" s="18" t="s">
-        <v>88</v>
+        <v>38</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>82</v>
       </c>
       <c r="E30" s="5"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D31" s="17" t="s">
-        <v>86</v>
+        <v>37</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>80</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D32" s="17" t="s">
-        <v>87</v>
+        <v>36</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>81</v>
       </c>
       <c r="E32" s="8"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B33" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C33" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D33" s="17" t="s">
-        <v>87</v>
+      <c r="D33" s="15" t="s">
+        <v>81</v>
       </c>
       <c r="E33" s="8"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D34" s="17" t="s">
-        <v>7</v>
+        <v>34</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>5</v>
       </c>
       <c r="E34" s="8"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D35" s="17" t="s">
-        <v>7</v>
+        <v>33</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>5</v>
       </c>
       <c r="E35" s="8"/>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D36" s="17" t="s">
-        <v>88</v>
+        <v>32</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>82</v>
       </c>
       <c r="E36" s="8"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D37" s="17" t="s">
-        <v>88</v>
+        <v>30</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>82</v>
       </c>
       <c r="E37" s="8"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D38" s="18" t="s">
-        <v>86</v>
+        <v>29</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>80</v>
       </c>
       <c r="E38" s="5"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D39" s="18" t="s">
-        <v>88</v>
+        <v>28</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>82</v>
       </c>
       <c r="E39" s="5"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D40" s="18" t="s">
-        <v>87</v>
+        <v>26</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>81</v>
       </c>
       <c r="E40" s="5"/>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B41" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C41" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D41" s="17" t="s">
-        <v>86</v>
+      <c r="D41" s="15" t="s">
+        <v>80</v>
       </c>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D42" s="17" t="s">
-        <v>87</v>
+        <v>24</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>81</v>
       </c>
       <c r="E42" s="8"/>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D43" s="17" t="s">
-        <v>7</v>
+        <v>23</v>
+      </c>
+      <c r="D43" s="15" t="s">
+        <v>5</v>
       </c>
       <c r="E43" s="8"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D44" s="17" t="s">
-        <v>7</v>
+        <v>22</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>5</v>
       </c>
       <c r="E44" s="8"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C45" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D45" s="17" t="s">
-        <v>88</v>
+      <c r="D45" s="15" t="s">
+        <v>82</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B46" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C46" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C46" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D46" s="18" t="s">
-        <v>86</v>
+      <c r="D46" s="16" t="s">
+        <v>80</v>
       </c>
       <c r="E46" s="5"/>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D47" s="18" t="s">
-        <v>87</v>
+        <v>19</v>
+      </c>
+      <c r="D47" s="16" t="s">
+        <v>81</v>
       </c>
       <c r="E47" s="5"/>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D48" s="18" t="s">
-        <v>7</v>
+        <v>18</v>
+      </c>
+      <c r="D48" s="16" t="s">
+        <v>5</v>
       </c>
       <c r="E48" s="5"/>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C49" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B49" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D49" s="18" t="s">
-        <v>88</v>
+      <c r="D49" s="16" t="s">
+        <v>82</v>
       </c>
       <c r="E49" s="5"/>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D50" s="18" t="s">
-        <v>88</v>
+        <v>15</v>
+      </c>
+      <c r="D50" s="16" t="s">
+        <v>82</v>
       </c>
       <c r="E50" s="5"/>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C51" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D51" s="17" t="s">
-        <v>88</v>
+      <c r="D51" s="15" t="s">
+        <v>82</v>
       </c>
       <c r="E51" s="8"/>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C52" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D52" s="17" t="s">
-        <v>86</v>
+      <c r="D52" s="15" t="s">
+        <v>80</v>
       </c>
       <c r="E52" s="8"/>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D53" s="19" t="s">
-        <v>86</v>
+        <v>10</v>
+      </c>
+      <c r="D53" s="17" t="s">
+        <v>80</v>
       </c>
       <c r="E53" s="3"/>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D54" s="19" t="s">
-        <v>87</v>
+        <v>9</v>
+      </c>
+      <c r="D54" s="17" t="s">
+        <v>81</v>
       </c>
       <c r="E54" s="3"/>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D55" s="19" t="s">
-        <v>88</v>
+        <v>8</v>
+      </c>
+      <c r="D55" s="17" t="s">
+        <v>82</v>
       </c>
       <c r="E55" s="3"/>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D56" s="19" t="s">
-        <v>88</v>
+        <v>7</v>
+      </c>
+      <c r="D56" s="17" t="s">
+        <v>82</v>
       </c>
       <c r="E56" s="3"/>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D57" s="19" t="s">
+      <c r="D57" s="17" t="s">
         <v>4</v>
       </c>
       <c r="E57" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D58" s="17" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" s="14" customFormat="1">
-      <c r="A58" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B58" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C58" s="13" t="s">
+      <c r="E58" s="3"/>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D59" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="E59" s="3"/>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D60" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E60" s="1"/>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D58" s="20"/>
-      <c r="E58" s="14" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" s="14" customFormat="1">
-      <c r="A59" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B59" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C59" s="13" t="s">
+      <c r="D61" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="E61" s="1"/>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D59" s="20"/>
-    </row>
-    <row r="60" spans="1:5" s="14" customFormat="1">
-      <c r="A60" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B60" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C60" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D60" s="20"/>
-    </row>
-    <row r="61" spans="1:5" s="14" customFormat="1">
-      <c r="A61" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B61" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C61" s="13" t="s">
+      <c r="D62" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="E62" s="1"/>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D61" s="20"/>
-    </row>
-    <row r="62" spans="1:5" s="14" customFormat="1">
-      <c r="A62" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B62" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C62" s="13" t="s">
+      <c r="C63" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D62" s="20" t="s">
+      <c r="D63" s="18" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="63" spans="1:5">
-      <c r="A63" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B63" s="4" t="s">
+      <c r="E63" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C63" s="4" t="s">
+      <c r="C64" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D63" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="E63" s="3"/>
-    </row>
-    <row r="64" spans="1:5">
-      <c r="A64" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D64" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="E64" s="3"/>
+      <c r="D64" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E64" s="1"/>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D65" s="21" t="s">
-        <v>86</v>
+        <v>0</v>
+      </c>
+      <c r="D65" s="18" t="s">
+        <v>82</v>
       </c>
       <c r="E65" s="1"/>
-    </row>
-    <row r="66" spans="1:5">
-      <c r="A66" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D66" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="E66" s="1"/>
-    </row>
-    <row r="67" spans="1:5">
-      <c r="A67" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D67" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="E67" s="1"/>
-    </row>
-    <row r="68" spans="1:5" s="14" customFormat="1">
-      <c r="A68" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B68" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C68" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D68" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="E68" s="14" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5">
-      <c r="A69" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D69" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" s="14" customFormat="1">
-      <c r="A70" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B70" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C70" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D70" s="20"/>
-      <c r="E70" s="14" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" s="14" customFormat="1">
-      <c r="A71" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B71" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C71" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D71" s="20"/>
-    </row>
-    <row r="72" spans="1:5" s="14" customFormat="1">
-      <c r="A72" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B72" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C72" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D72" s="20"/>
-    </row>
-    <row r="73" spans="1:5" s="14" customFormat="1">
-      <c r="A73" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B73" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C73" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D73" s="20"/>
-    </row>
-    <row r="74" spans="1:5" s="14" customFormat="1">
-      <c r="A74" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B74" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C74" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D74" s="20" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5">
-      <c r="A75" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D75" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="E75" s="1"/>
-    </row>
-    <row r="76" spans="1:5">
-      <c r="A76" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D76" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="E76" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
cleaning up traits and scoring sheets
</commit_message>
<xml_diff>
--- a/trait_stressor_rankings/trait_stressor_adcap_general.xlsx
+++ b/trait_stressor_rankings/trait_stressor_adcap_general.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4220" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="4860" yWindow="500" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="stressor1" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="93">
   <si>
     <t>no</t>
   </si>
@@ -288,6 +288,209 @@
   </si>
   <si>
     <t>lit review</t>
+  </si>
+  <si>
+    <r>
+      <t>Jennings et al (1999) demonstrated that "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>fishing has greater effects</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> on slower growing, larger species with later maturity and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>lower rates of potential population increase</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <t>Jennings et al (1999)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Species of macroalgae with extended reproductive period, either long continuous spore release, or vegetative dispersal, less sensitive to sedimentation (Eriksson &amp; Johansson 2005). 'The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>extended
+spawning period</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of C. foliascens [38], and concomitant </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>higher potential for larval supply</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, reflects patterns observed for abundant Red Sea sponges species Niphates sp. and Chalinula sp. [44,45].
+Year-round spawning is likely to be a factor contributing to the abundance of C. foliascens on the GBR where they can represent up to 80% of total sponge abundance and biomass' (Wahab et al 2014).</t>
+    </r>
+  </si>
+  <si>
+    <t>Eriksson &amp; Johansson (2005)(macroalgae), Wahab et al (2014)(sponge larvae)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"The results provide quantitative evidence to support speculation that fishing has had greater effects on slower growing, larger species with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>late maturity</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">" (Jennings et al 1999). Juan-Jorda et al (2015) found that growth rate and age at maturity better explained extent and rate of declines than max body size re their vulnerability to overfishing. "...there is strong geographical patterning in population declines, such that populations with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>slower life histories</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (found at higher cooler latitudes) have declined most and more steeply and have a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>higher probability of being overfished</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> than populations with faster life histories (found at tropical latitudes)." 'Adding to the vulnerability of this species is its </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>late maturity</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> at a large size (Hamilton et al. 2008) and the restriction of juvenile recruitment to lagoonal fringing reef environments with high coral cover that are sensitive to the effect of poor land-based practices' (Hamilton et al 2016).</t>
+    </r>
+  </si>
+  <si>
+    <t>Jennings et al (1999), Juan-Jorda et al (2015), Hamilton et al (2016)(reef fish)</t>
+  </si>
+  <si>
+    <t>"global warming will lead to an increasing dominance and geographical expansion of fast-growing, early-maturing and short-lived species" (Beukhof et al 2019)</t>
+  </si>
+  <si>
+    <t>Beukhof et al (2019)</t>
+  </si>
+  <si>
+    <t>"Heavily calcified single-celled animals, such as coccolithophores, have rapid generation times, and therefore the potential to adapt much more quickly to changing conditions than multicellular invertebrates (Schlüter et al., 2014)."(Clark 2020)</t>
   </si>
 </sst>
 </file>
@@ -381,7 +584,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -395,8 +598,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -418,20 +623,24 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -765,10 +974,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -779,7 +988,7 @@
     <col min="4" max="4" width="10.83203125" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="11" customFormat="1">
+    <row r="1" spans="1:6" s="11" customFormat="1">
       <c r="A1" s="12" t="s">
         <v>73</v>
       </c>
@@ -796,7 +1005,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" s="10" t="s">
         <v>63</v>
       </c>
@@ -812,8 +1021,9 @@
       <c r="E2" s="9" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="9"/>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="10" t="s">
         <v>63</v>
       </c>
@@ -827,8 +1037,9 @@
         <v>81</v>
       </c>
       <c r="E3" s="9"/>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" s="9"/>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="10" t="s">
         <v>63</v>
       </c>
@@ -842,8 +1053,9 @@
         <v>5</v>
       </c>
       <c r="E4" s="9"/>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="10" t="s">
         <v>63</v>
       </c>
@@ -857,8 +1069,9 @@
         <v>82</v>
       </c>
       <c r="E5" s="9"/>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" s="9"/>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="7" t="s">
         <v>13</v>
       </c>
@@ -874,8 +1087,9 @@
       <c r="E6" s="20" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" s="20"/>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="7" t="s">
         <v>13</v>
       </c>
@@ -886,13 +1100,14 @@
         <v>61</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" s="8"/>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="7" t="s">
         <v>13</v>
       </c>
@@ -903,11 +1118,12 @@
         <v>60</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>82</v>
+        <v>5</v>
       </c>
       <c r="E8" s="8"/>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -921,8 +1137,9 @@
         <v>82</v>
       </c>
       <c r="E9" s="8"/>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="7" t="s">
         <v>13</v>
       </c>
@@ -935,9 +1152,14 @@
       <c r="D10" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="E10" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -948,11 +1170,12 @@
         <v>57</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="7" t="s">
         <v>13</v>
       </c>
@@ -966,8 +1189,9 @@
         <v>81</v>
       </c>
       <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="7" t="s">
         <v>13</v>
       </c>
@@ -981,8 +1205,9 @@
         <v>81</v>
       </c>
       <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="7" t="s">
         <v>13</v>
       </c>
@@ -993,11 +1218,12 @@
         <v>54</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>81</v>
+        <v>5</v>
       </c>
       <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="7" t="s">
         <v>13</v>
       </c>
@@ -1011,8 +1237,9 @@
         <v>5</v>
       </c>
       <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="7" t="s">
         <v>13</v>
       </c>
@@ -1026,8 +1253,9 @@
         <v>5</v>
       </c>
       <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="7" t="s">
         <v>13</v>
       </c>
@@ -1041,8 +1269,9 @@
         <v>5</v>
       </c>
       <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="7" t="s">
         <v>13</v>
       </c>
@@ -1056,8 +1285,9 @@
         <v>82</v>
       </c>
       <c r="E18" s="5"/>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="7" t="s">
         <v>13</v>
       </c>
@@ -1071,8 +1301,9 @@
         <v>82</v>
       </c>
       <c r="E19" s="5"/>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="7" t="s">
         <v>13</v>
       </c>
@@ -1086,8 +1317,9 @@
         <v>80</v>
       </c>
       <c r="E20" s="8"/>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="F20" s="8"/>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="7" t="s">
         <v>13</v>
       </c>
@@ -1101,8 +1333,9 @@
         <v>81</v>
       </c>
       <c r="E21" s="8"/>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="F21" s="8"/>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="7" t="s">
         <v>13</v>
       </c>
@@ -1116,8 +1349,9 @@
         <v>81</v>
       </c>
       <c r="E22" s="8"/>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="F22" s="8"/>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="7" t="s">
         <v>13</v>
       </c>
@@ -1131,8 +1365,9 @@
         <v>5</v>
       </c>
       <c r="E23" s="8"/>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="F23" s="8"/>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="7" t="s">
         <v>13</v>
       </c>
@@ -1146,8 +1381,9 @@
         <v>5</v>
       </c>
       <c r="E24" s="8"/>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="F24" s="8"/>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="7" t="s">
         <v>13</v>
       </c>
@@ -1160,9 +1396,14 @@
       <c r="D25" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="E25" s="8"/>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="E25" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="7" t="s">
         <v>13</v>
       </c>
@@ -1175,9 +1416,14 @@
       <c r="D26" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="E26" s="5"/>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="E26" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" s="7" t="s">
         <v>13</v>
       </c>
@@ -1191,8 +1437,9 @@
         <v>81</v>
       </c>
       <c r="E27" s="5"/>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" s="7" t="s">
         <v>13</v>
       </c>
@@ -1206,8 +1453,9 @@
         <v>81</v>
       </c>
       <c r="E28" s="5"/>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" s="7" t="s">
         <v>13</v>
       </c>
@@ -1220,9 +1468,14 @@
       <c r="D29" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="E29" s="5"/>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="E29" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" s="7" t="s">
         <v>13</v>
       </c>
@@ -1235,9 +1488,12 @@
       <c r="D30" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="E30" s="5"/>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="E30" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" s="7" t="s">
         <v>13</v>
       </c>
@@ -1253,8 +1509,9 @@
       <c r="E31" s="8" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="F31" s="8"/>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" s="7" t="s">
         <v>13</v>
       </c>
@@ -1268,8 +1525,9 @@
         <v>81</v>
       </c>
       <c r="E32" s="8"/>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="F32" s="8"/>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="7" t="s">
         <v>13</v>
       </c>
@@ -1283,8 +1541,9 @@
         <v>81</v>
       </c>
       <c r="E33" s="8"/>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="F33" s="8"/>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="7" t="s">
         <v>13</v>
       </c>
@@ -1298,8 +1557,9 @@
         <v>5</v>
       </c>
       <c r="E34" s="8"/>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="F34" s="8"/>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" s="7" t="s">
         <v>13</v>
       </c>
@@ -1313,8 +1573,9 @@
         <v>5</v>
       </c>
       <c r="E35" s="8"/>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="F35" s="8"/>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" s="7" t="s">
         <v>13</v>
       </c>
@@ -1328,8 +1589,9 @@
         <v>82</v>
       </c>
       <c r="E36" s="8"/>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="F36" s="8"/>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" s="7" t="s">
         <v>13</v>
       </c>
@@ -1343,8 +1605,9 @@
         <v>82</v>
       </c>
       <c r="E37" s="8"/>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="F37" s="8"/>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" s="7" t="s">
         <v>13</v>
       </c>
@@ -1358,8 +1621,9 @@
         <v>80</v>
       </c>
       <c r="E38" s="5"/>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="F38" s="5"/>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" s="7" t="s">
         <v>13</v>
       </c>
@@ -1370,11 +1634,12 @@
         <v>28</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>82</v>
+        <v>5</v>
       </c>
       <c r="E39" s="5"/>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="F39" s="5"/>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" s="7" t="s">
         <v>13</v>
       </c>
@@ -1385,11 +1650,12 @@
         <v>26</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E40" s="5"/>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="F40" s="5"/>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" s="7" t="s">
         <v>13</v>
       </c>
@@ -1403,8 +1669,9 @@
         <v>80</v>
       </c>
       <c r="E41" s="8"/>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="F41" s="8"/>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" s="7" t="s">
         <v>13</v>
       </c>
@@ -1418,8 +1685,9 @@
         <v>81</v>
       </c>
       <c r="E42" s="8"/>
-    </row>
-    <row r="43" spans="1:5">
+      <c r="F42" s="8"/>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" s="7" t="s">
         <v>13</v>
       </c>
@@ -1433,8 +1701,9 @@
         <v>5</v>
       </c>
       <c r="E43" s="8"/>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="F43" s="8"/>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" s="7" t="s">
         <v>13</v>
       </c>
@@ -1448,8 +1717,9 @@
         <v>5</v>
       </c>
       <c r="E44" s="8"/>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="F44" s="8"/>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" s="7" t="s">
         <v>13</v>
       </c>
@@ -1465,8 +1735,9 @@
       <c r="E45" s="8" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="46" spans="1:5">
+      <c r="F45" s="8"/>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" s="7" t="s">
         <v>13</v>
       </c>
@@ -1480,8 +1751,9 @@
         <v>80</v>
       </c>
       <c r="E46" s="5"/>
-    </row>
-    <row r="47" spans="1:5">
+      <c r="F46" s="5"/>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" s="7" t="s">
         <v>13</v>
       </c>
@@ -1495,8 +1767,9 @@
         <v>81</v>
       </c>
       <c r="E47" s="5"/>
-    </row>
-    <row r="48" spans="1:5">
+      <c r="F47" s="5"/>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48" s="7" t="s">
         <v>13</v>
       </c>
@@ -1510,8 +1783,9 @@
         <v>5</v>
       </c>
       <c r="E48" s="5"/>
-    </row>
-    <row r="49" spans="1:5">
+      <c r="F48" s="5"/>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" s="7" t="s">
         <v>13</v>
       </c>
@@ -1522,11 +1796,12 @@
         <v>17</v>
       </c>
       <c r="D49" s="16" t="s">
-        <v>82</v>
+        <v>5</v>
       </c>
       <c r="E49" s="5"/>
-    </row>
-    <row r="50" spans="1:5">
+      <c r="F49" s="5"/>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" s="7" t="s">
         <v>13</v>
       </c>
@@ -1540,8 +1815,9 @@
         <v>82</v>
       </c>
       <c r="E50" s="5"/>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="F50" s="5"/>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" s="7" t="s">
         <v>13</v>
       </c>
@@ -1555,8 +1831,9 @@
         <v>82</v>
       </c>
       <c r="E51" s="8"/>
-    </row>
-    <row r="52" spans="1:5">
+      <c r="F51" s="8"/>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52" s="7" t="s">
         <v>13</v>
       </c>
@@ -1570,8 +1847,9 @@
         <v>80</v>
       </c>
       <c r="E52" s="8"/>
-    </row>
-    <row r="53" spans="1:5">
+      <c r="F52" s="8"/>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53" s="4" t="s">
         <v>11</v>
       </c>
@@ -1585,8 +1863,9 @@
         <v>80</v>
       </c>
       <c r="E53" s="3"/>
-    </row>
-    <row r="54" spans="1:5">
+      <c r="F53" s="3"/>
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54" s="4" t="s">
         <v>11</v>
       </c>
@@ -1600,8 +1879,9 @@
         <v>81</v>
       </c>
       <c r="E54" s="3"/>
-    </row>
-    <row r="55" spans="1:5">
+      <c r="F54" s="3"/>
+    </row>
+    <row r="55" spans="1:6">
       <c r="A55" s="4" t="s">
         <v>11</v>
       </c>
@@ -1615,8 +1895,9 @@
         <v>82</v>
       </c>
       <c r="E55" s="3"/>
-    </row>
-    <row r="56" spans="1:5">
+      <c r="F55" s="3"/>
+    </row>
+    <row r="56" spans="1:6">
       <c r="A56" s="4" t="s">
         <v>11</v>
       </c>
@@ -1630,8 +1911,9 @@
         <v>82</v>
       </c>
       <c r="E56" s="3"/>
-    </row>
-    <row r="57" spans="1:5">
+      <c r="F56" s="3"/>
+    </row>
+    <row r="57" spans="1:6">
       <c r="A57" s="4" t="s">
         <v>11</v>
       </c>
@@ -1647,8 +1929,9 @@
       <c r="E57" s="3" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="58" spans="1:5">
+      <c r="F57" s="3"/>
+    </row>
+    <row r="58" spans="1:6">
       <c r="A58" s="4" t="s">
         <v>11</v>
       </c>
@@ -1662,8 +1945,9 @@
         <v>80</v>
       </c>
       <c r="E58" s="3"/>
-    </row>
-    <row r="59" spans="1:5">
+      <c r="F58" s="3"/>
+    </row>
+    <row r="59" spans="1:6">
       <c r="A59" s="4" t="s">
         <v>11</v>
       </c>
@@ -1677,8 +1961,9 @@
         <v>82</v>
       </c>
       <c r="E59" s="3"/>
-    </row>
-    <row r="60" spans="1:5">
+      <c r="F59" s="3"/>
+    </row>
+    <row r="60" spans="1:6">
       <c r="A60" s="2" t="s">
         <v>2</v>
       </c>
@@ -1692,8 +1977,9 @@
         <v>80</v>
       </c>
       <c r="E60" s="1"/>
-    </row>
-    <row r="61" spans="1:5">
+      <c r="F60" s="1"/>
+    </row>
+    <row r="61" spans="1:6">
       <c r="A61" s="2" t="s">
         <v>2</v>
       </c>
@@ -1707,8 +1993,9 @@
         <v>81</v>
       </c>
       <c r="E61" s="1"/>
-    </row>
-    <row r="62" spans="1:5">
+      <c r="F61" s="1"/>
+    </row>
+    <row r="62" spans="1:6">
       <c r="A62" s="2" t="s">
         <v>2</v>
       </c>
@@ -1722,8 +2009,9 @@
         <v>82</v>
       </c>
       <c r="E62" s="1"/>
-    </row>
-    <row r="63" spans="1:5">
+      <c r="F62" s="1"/>
+    </row>
+    <row r="63" spans="1:6">
       <c r="A63" s="2" t="s">
         <v>2</v>
       </c>
@@ -1739,8 +2027,9 @@
       <c r="E63" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="64" spans="1:5">
+      <c r="F63" s="1"/>
+    </row>
+    <row r="64" spans="1:6">
       <c r="A64" s="2" t="s">
         <v>2</v>
       </c>
@@ -1754,8 +2043,9 @@
         <v>80</v>
       </c>
       <c r="E64" s="1"/>
-    </row>
-    <row r="65" spans="1:5">
+      <c r="F64" s="1"/>
+    </row>
+    <row r="65" spans="1:6">
       <c r="A65" s="2" t="s">
         <v>2</v>
       </c>
@@ -1769,6 +2059,7 @@
         <v>82</v>
       </c>
       <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>